<commit_message>
Added Conference Championship Predictions
</commit_message>
<xml_diff>
--- a/Playoff Predictions/Weekdiv_matrix.xlsx
+++ b/Playoff Predictions/Weekdiv_matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="1" r:id="rId1"/>
@@ -552,15 +552,99 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,90 +661,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3158,7 +3158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -3519,7 +3519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -3573,17 +3573,17 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="14"/>
+      <c r="I2" s="43"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
-      <c r="P2" s="15"/>
+      <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="11"/>
@@ -3593,17 +3593,17 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="45"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
-      <c r="P3" s="15"/>
+      <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
@@ -3613,17 +3613,17 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="19"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
-      <c r="P4" s="15"/>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11"/>
@@ -3633,17 +3633,17 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
-      <c r="P5" s="15"/>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11"/>
@@ -3654,14 +3654,14 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="22"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-      <c r="P6" s="15"/>
+      <c r="P6" s="13"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11"/>
@@ -3671,10 +3671,10 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="16" t="s">
         <v>25</v>
       </c>
       <c r="J7" s="12"/>
@@ -3683,7 +3683,7 @@
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
-      <c r="P7" s="15"/>
+      <c r="P7" s="13"/>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11"/>
@@ -3691,21 +3691,21 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27">
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19">
         <v>21</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="20">
         <v>20</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="23"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
-      <c r="P8" s="15"/>
+      <c r="P8" s="13"/>
     </row>
     <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11"/>
@@ -3714,10 +3714,10 @@
       <c r="D9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="24" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="12" t="s">
@@ -3728,234 +3728,234 @@
       <c r="J9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="25" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
-      <c r="P9" s="15"/>
+      <c r="P9" s="13"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27">
+      <c r="C10" s="26"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19">
         <v>28</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="20">
         <v>27</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
-      <c r="K10" s="27">
+      <c r="K10" s="19">
         <v>23</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="20">
         <v>23</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="15"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="31"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="22"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
-      <c r="L11" s="22"/>
+      <c r="L11" s="14"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="15"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="13"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11"/>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="28" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="29" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="42" t="s">
+      <c r="L12" s="34" t="s">
         <v>34</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O12" s="39" t="s">
+      <c r="O12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="15"/>
+      <c r="P12" s="13"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11"/>
-      <c r="B13" s="27">
+      <c r="B13" s="19">
         <v>24</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="20">
         <v>21</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="27">
+      <c r="E13" s="19">
         <v>30</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="20">
         <v>27</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="27">
+      <c r="K13" s="19">
         <v>24</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="20">
         <v>13</v>
       </c>
       <c r="M13" s="12"/>
-      <c r="N13" s="27">
+      <c r="N13" s="19">
         <v>28</v>
       </c>
-      <c r="O13" s="28">
+      <c r="O13" s="20">
         <v>27</v>
       </c>
-      <c r="P13" s="15"/>
+      <c r="P13" s="13"/>
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="22"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
-      <c r="L14" s="22"/>
+      <c r="L14" s="14"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="15"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="13"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="11"/>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="28" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="12"/>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="33" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
-      <c r="K15" s="42" t="s">
+      <c r="K15" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="30" t="s">
         <v>30</v>
       </c>
       <c r="M15" s="12"/>
-      <c r="N15" s="39" t="s">
+      <c r="N15" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="O15" s="43" t="s">
+      <c r="O15" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="P15" s="15"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="11"/>
-      <c r="B16" s="47">
+      <c r="B16" s="39">
         <v>17</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="40">
         <v>30</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="48">
+      <c r="D16" s="41"/>
+      <c r="E16" s="40">
         <v>26</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="39">
         <v>10</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="48">
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="40">
         <v>27</v>
       </c>
-      <c r="L16" s="47">
+      <c r="L16" s="39">
         <v>16</v>
       </c>
-      <c r="M16" s="49"/>
-      <c r="N16" s="48">
+      <c r="M16" s="41"/>
+      <c r="N16" s="40">
         <v>24</v>
       </c>
-      <c r="O16" s="47">
+      <c r="O16" s="39">
         <v>20</v>
       </c>
-      <c r="P16" s="15"/>
+      <c r="P16" s="13"/>
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="46"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>